<commit_message>
Update readme.md and tesing matrix
Elaborate on deployment, testing and features sections
of the readme.md to provide a more in depth documentation.
</commit_message>
<xml_diff>
--- a/docs/testing.xlsx
+++ b/docs/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bushm\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07737775-47FE-4917-BC5D-85931B929A9D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F1337B-BA2D-4AC7-A54A-7DD3C060BE76}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="48">
   <si>
     <t>Firefox</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t xml:space="preserve">✔ </t>
+  </si>
+  <si>
+    <t>Intro.js</t>
+  </si>
+  <si>
+    <t>Runs when "take tutorial" is clicked in modal</t>
+  </si>
+  <si>
+    <t>Runs when "question" icon is clicked</t>
   </si>
 </sst>
 </file>
@@ -976,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="11.5" x14ac:dyDescent="0.3"/>
@@ -1171,14 +1180,18 @@
       <c r="L9" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="12"/>
+      <c r="M9" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N9" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O9" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P9" s="12"/>
+      <c r="P9" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:16" s="17" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
@@ -1215,14 +1228,18 @@
       <c r="L10" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="M10" s="11"/>
+      <c r="M10" s="29" t="s">
+        <v>40</v>
+      </c>
       <c r="N10" s="29" t="s">
         <v>40</v>
       </c>
       <c r="O10" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="P10" s="11"/>
+      <c r="P10" s="29" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1258,14 +1275,18 @@
       <c r="L11" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M11" s="12"/>
+      <c r="M11" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N11" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O11" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P11" s="12"/>
+      <c r="P11" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1301,14 +1322,18 @@
       <c r="L12" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M12" s="12"/>
+      <c r="M12" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N12" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O12" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P12" s="12"/>
+      <c r="P12" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1344,14 +1369,18 @@
       <c r="L13" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M13" s="12"/>
+      <c r="M13" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N13" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O13" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P13" s="12"/>
+      <c r="P13" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -1387,14 +1416,18 @@
       <c r="L14" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M14" s="12"/>
+      <c r="M14" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N14" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O14" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P14" s="12"/>
+      <c r="P14" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1430,14 +1463,18 @@
       <c r="L15" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M15" s="12"/>
+      <c r="M15" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N15" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O15" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P15" s="12"/>
+      <c r="P15" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -1473,14 +1510,18 @@
       <c r="L16" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M16" s="12"/>
+      <c r="M16" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N16" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O16" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P16" s="12"/>
+      <c r="P16" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="17" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
@@ -1496,10 +1537,10 @@
       <c r="J17" s="27"/>
       <c r="K17" s="27"/>
       <c r="L17" s="27"/>
-      <c r="M17" s="3"/>
+      <c r="M17" s="27"/>
       <c r="N17" s="27"/>
       <c r="O17" s="27"/>
-      <c r="P17" s="3"/>
+      <c r="P17" s="27"/>
     </row>
     <row r="18" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -1535,14 +1576,18 @@
       <c r="L18" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M18" s="12"/>
+      <c r="M18" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N18" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O18" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P18" s="12"/>
+      <c r="P18" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="19" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -1578,14 +1623,18 @@
       <c r="L19" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M19" s="12"/>
+      <c r="M19" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N19" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O19" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P19" s="12"/>
+      <c r="P19" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="20" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -1621,14 +1670,18 @@
       <c r="L20" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M20" s="12"/>
+      <c r="M20" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N20" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O20" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P20" s="12"/>
+      <c r="P20" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
@@ -1644,10 +1697,10 @@
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
-      <c r="M21" s="3"/>
+      <c r="M21" s="27"/>
       <c r="N21" s="27"/>
       <c r="O21" s="27"/>
-      <c r="P21" s="3"/>
+      <c r="P21" s="27"/>
     </row>
     <row r="22" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1683,14 +1736,18 @@
       <c r="L22" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M22" s="12"/>
+      <c r="M22" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N22" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O22" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P22" s="12"/>
+      <c r="P22" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="23" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -1726,14 +1783,18 @@
       <c r="L23" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M23" s="12"/>
+      <c r="M23" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N23" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O23" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P23" s="12"/>
+      <c r="P23" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="24" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
@@ -1749,10 +1810,10 @@
       <c r="J24" s="27"/>
       <c r="K24" s="27"/>
       <c r="L24" s="27"/>
-      <c r="M24" s="3"/>
+      <c r="M24" s="27"/>
       <c r="N24" s="27"/>
       <c r="O24" s="27"/>
-      <c r="P24" s="3"/>
+      <c r="P24" s="27"/>
     </row>
     <row r="25" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
@@ -1788,14 +1849,18 @@
       <c r="L25" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M25" s="12"/>
+      <c r="M25" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N25" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O25" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P25" s="12"/>
+      <c r="P25" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="26" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -1831,14 +1896,18 @@
       <c r="L26" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M26" s="12"/>
+      <c r="M26" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N26" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O26" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P26" s="12"/>
+      <c r="P26" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="27" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -1874,14 +1943,18 @@
       <c r="L27" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M27" s="12"/>
+      <c r="M27" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N27" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O27" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P27" s="12"/>
+      <c r="P27" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -1918,81 +1991,237 @@
       <c r="L28" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M28" s="12"/>
+      <c r="M28" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="N28" s="26" t="s">
         <v>40</v>
       </c>
       <c r="O28" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P28" s="12"/>
+      <c r="P28" s="26" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="29" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="A29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
     </row>
     <row r="30" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="L30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="M30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="O30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="P30" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J31" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="L31" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="M31" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N31" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="O31" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="P31" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K32" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="M32" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N32" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="O32" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="P32" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="30"/>
-    </row>
-    <row r="31" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="40" t="s">
+      <c r="B34" s="38"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="30"/>
+    </row>
+    <row r="35" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+      <c r="A35" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="42"/>
-    </row>
-    <row r="32" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="31"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="33"/>
-    </row>
-    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="11"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="42"/>
+    </row>
+    <row r="36" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+      <c r="A36" s="31"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="33"/>
+    </row>
+    <row r="37" spans="1:7" ht="14" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="16"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A36:G36"/>
     <mergeCell ref="I6:P6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="A35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update testing for reset links
</commit_message>
<xml_diff>
--- a/docs/testing.xlsx
+++ b/docs/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bushm\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F1337B-BA2D-4AC7-A54A-7DD3C060BE76}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A9F1B0-9CAC-476A-A984-82B357557815}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,12 +85,6 @@
     <t xml:space="preserve">Grid is set appropraitely for screen size </t>
   </si>
   <si>
-    <t>Crimes Map reset link shows when map is clicked</t>
-  </si>
-  <si>
-    <t>Crimes Map reset link resets choropleth map and crimes row chart</t>
-  </si>
-  <si>
     <t>"Reset All" button link redraws all charts</t>
   </si>
   <si>
@@ -164,6 +158,12 @@
   </si>
   <si>
     <t>Runs when "question" icon is clicked</t>
+  </si>
+  <si>
+    <t>All reset links shows when charts are clicked (except for scatter plot and line chart)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All reset links remove all filters when it is clicked </t>
   </si>
 </sst>
 </file>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="11.5" x14ac:dyDescent="0.3"/>
@@ -1017,7 +1017,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -1030,7 +1030,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -1043,7 +1043,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1063,7 +1063,7 @@
     <row r="6" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -1072,7 +1072,7 @@
       <c r="G6" s="30"/>
       <c r="H6" s="21"/>
       <c r="I6" s="34" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
@@ -1085,25 +1085,25 @@
     <row r="7" spans="1:16" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="E7" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="F7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>39</v>
-      </c>
       <c r="G7" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J7" s="18" t="s">
         <v>0</v>
@@ -1118,13 +1118,13 @@
         <v>2</v>
       </c>
       <c r="N7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="18" t="s">
         <v>31</v>
-      </c>
-      <c r="O7" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="P7" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="17" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.3">
@@ -1151,46 +1151,46 @@
         <v>11</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N9" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O9" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="17" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1198,94 +1198,94 @@
         <v>12</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L10" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M10" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N10" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O10" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P10" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J11" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L11" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M11" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N11" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O11" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
@@ -1293,46 +1293,46 @@
         <v>13</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M12" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N12" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O12" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P12" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
@@ -1340,187 +1340,187 @@
         <v>14</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K13" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L13" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M13" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N13" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O13" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P13" s="26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="26.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L14" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M14" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N14" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O14" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P14" s="26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I15" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L15" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M15" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N15" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O15" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P15" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M16" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N16" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O16" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P16" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
@@ -1547,46 +1547,46 @@
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J18" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L18" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M18" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N18" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O18" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P18" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
@@ -1594,46 +1594,46 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I19" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K19" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L19" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M19" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N19" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O19" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P19" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
@@ -1641,46 +1641,46 @@
         <v>18</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J20" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K20" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M20" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N20" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O20" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P20" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
@@ -1707,46 +1707,46 @@
         <v>6</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J22" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K22" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L22" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M22" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N22" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O22" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P22" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
@@ -1754,51 +1754,51 @@
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I23" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J23" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K23" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L23" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M23" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N23" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O23" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1817,196 +1817,196 @@
     </row>
     <row r="25" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I25" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K25" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L25" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M25" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N25" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O25" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P25" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I26" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J26" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K26" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L26" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M26" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N26" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O26" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P26" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I27" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J27" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K27" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L27" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M27" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N27" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O27" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P27" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H28" s="23"/>
       <c r="I28" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J28" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K28" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L28" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M28" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N28" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O28" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P28" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2025,143 +2025,143 @@
     </row>
     <row r="30" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J30" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K30" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L30" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M30" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N30" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P30" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I31" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J31" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K31" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L31" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M31" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N31" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O31" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P31" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I32" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K32" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L32" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M32" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N32" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O32" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P32" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2178,7 +2178,7 @@
     </row>
     <row r="35" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A35" s="40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B35" s="41"/>
       <c r="C35" s="41"/>

</xml_diff>